<commit_message>
media queries fix, title dynamic
</commit_message>
<xml_diff>
--- a/public/movies.xlsx
+++ b/public/movies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GOOD show_locations_static" sheetId="1" r:id="rId1"/>
@@ -11510,7 +11510,7 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
@@ -11545,7 +11545,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="9">
-        <v>43970</v>
+        <v>43971</v>
       </c>
       <c r="D2" s="5">
         <v>0.63194444444444442</v>
@@ -11664,7 +11664,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="9">
-        <v>43970</v>
+        <v>43971</v>
       </c>
       <c r="D9" s="5">
         <v>0.61805555555555558</v>
@@ -11936,7 +11936,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="9">
-        <v>43970</v>
+        <v>43971</v>
       </c>
       <c r="D25" s="5">
         <v>0.60416666666666663</v>
@@ -12038,7 +12038,7 @@
         <v>19</v>
       </c>
       <c r="C31" s="9">
-        <v>43970</v>
+        <v>43971</v>
       </c>
       <c r="D31" s="5">
         <v>0.76388888888888884</v>
@@ -12259,7 +12259,7 @@
         <v>200</v>
       </c>
       <c r="C44" s="9">
-        <v>43970</v>
+        <v>43971</v>
       </c>
       <c r="D44" s="5">
         <v>0.47569444444444442</v>
@@ -12327,7 +12327,7 @@
         <v>200</v>
       </c>
       <c r="C48" s="9">
-        <v>43970</v>
+        <v>43971</v>
       </c>
       <c r="D48" s="5">
         <v>0.47916666666666669</v>
@@ -18078,7 +18078,7 @@
   </sheetPr>
   <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix city search duplicate
</commit_message>
<xml_diff>
--- a/public/movies.xlsx
+++ b/public/movies.xlsx
@@ -11510,7 +11510,7 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
@@ -11545,7 +11545,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="9">
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="D2" s="5">
         <v>0.63194444444444442</v>
@@ -11664,7 +11664,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="9">
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="D9" s="5">
         <v>0.61805555555555558</v>
@@ -11936,7 +11936,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="9">
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="D25" s="5">
         <v>0.60416666666666663</v>
@@ -12038,7 +12038,7 @@
         <v>19</v>
       </c>
       <c r="C31" s="9">
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="D31" s="5">
         <v>0.76388888888888884</v>
@@ -12259,7 +12259,7 @@
         <v>200</v>
       </c>
       <c r="C44" s="9">
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="D44" s="5">
         <v>0.47569444444444442</v>
@@ -12327,7 +12327,7 @@
         <v>200</v>
       </c>
       <c r="C48" s="9">
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="D48" s="5">
         <v>0.47916666666666669</v>
@@ -18078,7 +18078,7 @@
   </sheetPr>
   <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>

</xml_diff>